<commit_message>
fix bugs, modify codes
</commit_message>
<xml_diff>
--- a/uploads/2021_example_primary_school_completed.xlsx
+++ b/uploads/2021_example_primary_school_completed.xlsx
@@ -1066,7 +1066,7 @@
       </c>
       <c r="G7" s="11" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>Continuing</t>
         </is>
       </c>
       <c r="H7" s="11" t="inlineStr">
@@ -1093,12 +1093,20 @@
       <c r="O7" s="30" t="n">
         <v>0</v>
       </c>
-      <c r="P7" s="30" t="n"/>
-      <c r="Q7" s="30" t="n"/>
-      <c r="R7" s="30" t="n"/>
-      <c r="S7" s="30" t="n"/>
+      <c r="P7" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="30" t="n">
+        <v>5</v>
+      </c>
+      <c r="R7" s="30" t="n">
+        <v>9</v>
+      </c>
+      <c r="S7" s="30" t="n">
+        <v>13</v>
+      </c>
       <c r="T7" s="30" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="U7" s="13" t="inlineStr"/>
       <c r="V7" s="13" t="inlineStr"/>
@@ -1107,6 +1115,11 @@
           <t>attend</t>
         </is>
       </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>attend</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="24.75" customHeight="1" s="31">
       <c r="A8" s="30" t="n">
@@ -1137,7 +1150,7 @@
       </c>
       <c r="G8" s="11" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>Continuing</t>
         </is>
       </c>
       <c r="H8" s="11" t="inlineStr"/>
@@ -1162,22 +1175,35 @@
         <v>1</v>
       </c>
       <c r="O8" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" s="30" t="n"/>
-      <c r="Q8" s="30" t="n"/>
-      <c r="R8" s="30" t="n"/>
-      <c r="S8" s="30" t="n"/>
+        <v>20</v>
+      </c>
+      <c r="P8" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="R8" s="30" t="n">
+        <v>10</v>
+      </c>
+      <c r="S8" s="30" t="n">
+        <v>14</v>
+      </c>
       <c r="T8" s="30" t="n">
-        <v>20</v>
-      </c>
-      <c r="U8" s="13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="V8" s="13" t="inlineStr"/>
+        <v>34</v>
+      </c>
+      <c r="U8" s="13" t="inlineStr"/>
+      <c r="V8" s="13" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
       <c r="X8" t="inlineStr">
+        <is>
+          <t>attend</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
         <is>
           <t>attend</t>
         </is>
@@ -1237,17 +1263,30 @@
         <v>1</v>
       </c>
       <c r="O9" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="30" t="n"/>
-      <c r="Q9" s="30" t="n"/>
-      <c r="R9" s="30" t="n"/>
-      <c r="S9" s="30" t="n"/>
+        <v>20</v>
+      </c>
+      <c r="P9" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="30" t="n">
+        <v>7</v>
+      </c>
+      <c r="R9" s="30" t="n">
+        <v>11</v>
+      </c>
+      <c r="S9" s="30" t="n">
+        <v>15</v>
+      </c>
       <c r="T9" s="30" t="n">
-        <v>20</v>
-      </c>
-      <c r="U9" s="13" t="n"/>
-      <c r="V9" s="13" t="n"/>
+        <v>35</v>
+      </c>
+      <c r="U9" s="13" t="inlineStr"/>
+      <c r="V9" s="13" t="inlineStr"/>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>attend</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="24.75" customHeight="1" s="31">
       <c r="A10" s="30" t="n">
@@ -1303,14 +1342,27 @@
         <v>0</v>
       </c>
       <c r="O10" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" s="30" t="n"/>
-      <c r="Q10" s="30" t="n"/>
-      <c r="R10" s="30" t="n"/>
-      <c r="S10" s="30" t="n"/>
+        <v>20</v>
+      </c>
+      <c r="P10" s="30" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="30" t="n">
+        <v>8</v>
+      </c>
+      <c r="R10" s="30" t="n">
+        <v>12</v>
+      </c>
+      <c r="S10" s="30" t="n">
+        <v>16</v>
+      </c>
       <c r="T10" s="30" t="n">
-        <v>20</v>
+        <v>36</v>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>xl</t>
+        </is>
       </c>
       <c r="W10" t="inlineStr">
         <is>
@@ -1318,6 +1370,11 @@
         </is>
       </c>
       <c r="X10" t="inlineStr">
+        <is>
+          <t>attend</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
         <is>
           <t>attend</t>
         </is>
@@ -1352,7 +1409,7 @@
       </c>
       <c r="G11" s="13" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>Continuing</t>
         </is>
       </c>
       <c r="H11" s="13" t="inlineStr"/>
@@ -1377,16 +1434,34 @@
         <v>0</v>
       </c>
       <c r="O11" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" s="30" t="n"/>
-      <c r="Q11" s="30" t="n"/>
-      <c r="R11" s="30" t="n"/>
-      <c r="S11" s="30" t="n"/>
+        <v>20</v>
+      </c>
+      <c r="P11" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="30" t="n">
+        <v>5</v>
+      </c>
+      <c r="R11" s="30" t="n">
+        <v>9</v>
+      </c>
+      <c r="S11" s="30" t="n">
+        <v>13</v>
+      </c>
       <c r="T11" s="30" t="n">
-        <v>20</v>
+        <v>33</v>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
       </c>
       <c r="W11" t="inlineStr">
+        <is>
+          <t>attend</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr">
         <is>
           <t>attend</t>
         </is>
@@ -1446,14 +1521,32 @@
         <v>1</v>
       </c>
       <c r="O12" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" s="30" t="n"/>
-      <c r="Q12" s="30" t="n"/>
-      <c r="R12" s="30" t="n"/>
-      <c r="S12" s="30" t="n"/>
+        <v>20</v>
+      </c>
+      <c r="P12" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="R12" s="30" t="n">
+        <v>10</v>
+      </c>
+      <c r="S12" s="30" t="n">
+        <v>14</v>
+      </c>
       <c r="T12" s="30" t="n">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>xl</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>attend</t>
+        </is>
       </c>
     </row>
     <row r="13" ht="24.75" customHeight="1" s="31">
@@ -1485,7 +1578,7 @@
       </c>
       <c r="G13" s="13" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>Continuing</t>
         </is>
       </c>
       <c r="H13" s="13" t="inlineStr"/>
@@ -1510,14 +1603,22 @@
         <v>1</v>
       </c>
       <c r="O13" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" s="30" t="n"/>
-      <c r="Q13" s="30" t="n"/>
-      <c r="R13" s="30" t="n"/>
-      <c r="S13" s="30" t="n"/>
+        <v>20</v>
+      </c>
+      <c r="P13" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="30" t="n">
+        <v>7</v>
+      </c>
+      <c r="R13" s="30" t="n">
+        <v>11</v>
+      </c>
+      <c r="S13" s="30" t="n">
+        <v>15</v>
+      </c>
       <c r="T13" s="30" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="X13" t="inlineStr">
         <is>
@@ -1579,16 +1680,34 @@
         <v>1</v>
       </c>
       <c r="O14" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" s="30" t="n"/>
-      <c r="Q14" s="30" t="n"/>
-      <c r="R14" s="30" t="n"/>
-      <c r="S14" s="30" t="n"/>
+        <v>20</v>
+      </c>
+      <c r="P14" s="30" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="30" t="n">
+        <v>8</v>
+      </c>
+      <c r="R14" s="30" t="n">
+        <v>12</v>
+      </c>
+      <c r="S14" s="30" t="n">
+        <v>16</v>
+      </c>
       <c r="T14" s="30" t="n">
-        <v>20</v>
+        <v>36</v>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
       </c>
       <c r="W14" t="inlineStr">
+        <is>
+          <t>attend</t>
+        </is>
+      </c>
+      <c r="Z14" t="inlineStr">
         <is>
           <t>attend</t>
         </is>
@@ -1623,7 +1742,7 @@
       </c>
       <c r="G15" s="13" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>Continuing</t>
         </is>
       </c>
       <c r="H15" s="13" t="inlineStr"/>
@@ -1648,14 +1767,27 @@
         <v>0</v>
       </c>
       <c r="O15" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P15" s="30" t="n"/>
-      <c r="Q15" s="30" t="n"/>
-      <c r="R15" s="30" t="n"/>
-      <c r="S15" s="30" t="n"/>
+        <v>20</v>
+      </c>
+      <c r="P15" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="30" t="n">
+        <v>5</v>
+      </c>
+      <c r="R15" s="30" t="n">
+        <v>9</v>
+      </c>
+      <c r="S15" s="30" t="n">
+        <v>13</v>
+      </c>
       <c r="T15" s="30" t="n">
-        <v>20</v>
+        <v>33</v>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
       </c>
       <c r="W15" t="inlineStr">
         <is>
@@ -1722,14 +1854,27 @@
         <v>0</v>
       </c>
       <c r="O16" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P16" s="30" t="n"/>
-      <c r="Q16" s="30" t="n"/>
-      <c r="R16" s="30" t="n"/>
-      <c r="S16" s="30" t="n"/>
+        <v>20</v>
+      </c>
+      <c r="P16" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="R16" s="30" t="n">
+        <v>10</v>
+      </c>
+      <c r="S16" s="30" t="n">
+        <v>14</v>
+      </c>
       <c r="T16" s="30" t="n">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>attend</t>
+        </is>
       </c>
     </row>
     <row r="17" ht="24.75" customHeight="1" s="31">
@@ -1786,14 +1931,32 @@
         <v>1</v>
       </c>
       <c r="O17" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P17" s="30" t="n"/>
-      <c r="Q17" s="30" t="n"/>
-      <c r="R17" s="30" t="n"/>
-      <c r="S17" s="30" t="n"/>
+        <v>20</v>
+      </c>
+      <c r="P17" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="30" t="n">
+        <v>7</v>
+      </c>
+      <c r="R17" s="30" t="n">
+        <v>11</v>
+      </c>
+      <c r="S17" s="30" t="n">
+        <v>15</v>
+      </c>
       <c r="T17" s="30" t="n">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>attend</t>
+        </is>
       </c>
     </row>
     <row r="18" ht="24.75" customHeight="1" s="31">
@@ -1825,7 +1988,7 @@
       </c>
       <c r="G18" s="13" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>Continuing</t>
         </is>
       </c>
       <c r="H18" s="13" t="inlineStr"/>
@@ -1850,14 +2013,27 @@
         <v>1</v>
       </c>
       <c r="O18" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" s="30" t="n"/>
-      <c r="Q18" s="30" t="n"/>
-      <c r="R18" s="30" t="n"/>
-      <c r="S18" s="30" t="n"/>
+        <v>20</v>
+      </c>
+      <c r="P18" s="30" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q18" s="30" t="n">
+        <v>8</v>
+      </c>
+      <c r="R18" s="30" t="n">
+        <v>12</v>
+      </c>
+      <c r="S18" s="30" t="n">
+        <v>16</v>
+      </c>
       <c r="T18" s="30" t="n">
-        <v>20</v>
+        <v>36</v>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
       </c>
       <c r="W18" t="inlineStr">
         <is>
@@ -1924,14 +2100,22 @@
         <v>1</v>
       </c>
       <c r="O19" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P19" s="30" t="n"/>
-      <c r="Q19" s="30" t="n"/>
-      <c r="R19" s="30" t="n"/>
-      <c r="S19" s="30" t="n"/>
+        <v>20</v>
+      </c>
+      <c r="P19" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="30" t="n">
+        <v>5</v>
+      </c>
+      <c r="R19" s="30" t="n">
+        <v>9</v>
+      </c>
+      <c r="S19" s="30" t="n">
+        <v>13</v>
+      </c>
       <c r="T19" s="30" t="n">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="W19" t="inlineStr">
         <is>
@@ -1993,16 +2177,34 @@
         <v>0</v>
       </c>
       <c r="O20" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P20" s="30" t="n"/>
-      <c r="Q20" s="30" t="n"/>
-      <c r="R20" s="30" t="n"/>
-      <c r="S20" s="30" t="n"/>
+        <v>20</v>
+      </c>
+      <c r="P20" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="R20" s="30" t="n">
+        <v>10</v>
+      </c>
+      <c r="S20" s="30" t="n">
+        <v>14</v>
+      </c>
       <c r="T20" s="30" t="n">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
       </c>
       <c r="X20" t="inlineStr">
+        <is>
+          <t>attend</t>
+        </is>
+      </c>
+      <c r="Z20" t="inlineStr">
         <is>
           <t>attend</t>
         </is>
@@ -2037,7 +2239,7 @@
       </c>
       <c r="G21" s="13" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>Continuing</t>
         </is>
       </c>
       <c r="H21" s="13" t="inlineStr"/>
@@ -2062,14 +2264,22 @@
         <v>0</v>
       </c>
       <c r="O21" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P21" s="30" t="n"/>
-      <c r="Q21" s="30" t="n"/>
-      <c r="R21" s="30" t="n"/>
-      <c r="S21" s="30" t="n"/>
+        <v>20</v>
+      </c>
+      <c r="P21" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="30" t="n">
+        <v>7</v>
+      </c>
+      <c r="R21" s="30" t="n">
+        <v>11</v>
+      </c>
+      <c r="S21" s="30" t="n">
+        <v>15</v>
+      </c>
       <c r="T21" s="30" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" ht="24.75" customHeight="1" s="31">
@@ -2126,32 +2336,110 @@
         <v>1</v>
       </c>
       <c r="O22" s="30" t="n">
+        <v>20</v>
+      </c>
+      <c r="P22" s="30" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="30" t="n">
+        <v>8</v>
+      </c>
+      <c r="R22" s="30" t="n">
+        <v>12</v>
+      </c>
+      <c r="S22" s="30" t="n">
+        <v>16</v>
+      </c>
+      <c r="T22" s="30" t="n">
+        <v>36</v>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>attend</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="24.75" customHeight="1" s="31">
+      <c r="A23" s="30" t="n">
+        <v>100228</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>hhhhh</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>hhhhh</t>
+        </is>
+      </c>
+      <c r="D23" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Girl </t>
+        </is>
+      </c>
+      <c r="E23" s="30" t="n">
+        <v>11</v>
+      </c>
+      <c r="F23" s="13" t="inlineStr">
+        <is>
+          <t>European / Pākehā</t>
+        </is>
+      </c>
+      <c r="G23" s="13" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="H23" s="13" t="inlineStr"/>
+      <c r="I23" s="13" t="inlineStr">
+        <is>
+          <t>NZ00688</t>
+        </is>
+      </c>
+      <c r="J23" s="36" t="n">
+        <v>43896</v>
+      </c>
+      <c r="K23" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L23" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="M23" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N23" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O23" s="30" t="n">
         <v>0</v>
       </c>
-      <c r="P22" s="30" t="n"/>
-      <c r="Q22" s="30" t="n"/>
-      <c r="R22" s="30" t="n"/>
-      <c r="S22" s="30" t="n"/>
-      <c r="T22" s="30" t="n"/>
-    </row>
-    <row r="23" ht="24.75" customHeight="1" s="31">
-      <c r="A23" s="30" t="n"/>
-      <c r="D23" s="12" t="n"/>
-      <c r="E23" s="30" t="n"/>
-      <c r="F23" s="13" t="n"/>
-      <c r="G23" s="13" t="n"/>
-      <c r="H23" s="13" t="n"/>
-      <c r="I23" s="13" t="n"/>
-      <c r="K23" s="12" t="n"/>
-      <c r="L23" s="12" t="n"/>
-      <c r="M23" s="12" t="n"/>
-      <c r="N23" s="12" t="n"/>
-      <c r="O23" s="30" t="n"/>
-      <c r="P23" s="30" t="n"/>
-      <c r="Q23" s="30" t="n"/>
-      <c r="R23" s="30" t="n"/>
-      <c r="S23" s="30" t="n"/>
-      <c r="T23" s="30" t="n"/>
+      <c r="P23" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q23" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="R23" s="30" t="n">
+        <v>10</v>
+      </c>
+      <c r="S23" s="30" t="n">
+        <v>14</v>
+      </c>
+      <c r="T23" s="30" t="n">
+        <v>14</v>
+      </c>
+      <c r="Z23" t="inlineStr">
+        <is>
+          <t>attend</t>
+        </is>
+      </c>
     </row>
     <row r="24" ht="24.75" customHeight="1" s="31">
       <c r="A24" s="30" t="n"/>
@@ -16090,6 +16378,28 @@
       <c r="D22" t="inlineStr">
         <is>
           <t>asdfasdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>hhhhh</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>hhhhh</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>hhhhh</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>hhhhh</t>
         </is>
       </c>
     </row>
@@ -17391,7 +17701,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17445,13 +17755,21 @@
           <t>Smith</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="D2" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>100213</v>
+        <v>100187</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -17464,11 +17782,11 @@
         </is>
       </c>
       <c r="D3" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>term1</t>
+          <t>term2</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -17477,7 +17795,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>100213</v>
+        <v>100187</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -17490,20 +17808,20 @@
         </is>
       </c>
       <c r="D4" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>term2</t>
+          <t>term3</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>100213</v>
+        <v>100187</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -17516,15 +17834,15 @@
         </is>
       </c>
       <c r="D5" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>term3</t>
+          <t>term4</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
@@ -17542,63 +17860,63 @@
         </is>
       </c>
       <c r="D6" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>term4</t>
+          <t>term1</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>100214</v>
+        <v>100213</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Daisey</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Flower</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D7" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>term1</t>
+          <t>term2</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>100214</v>
+        <v>100213</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Daisey</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Flower</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D8" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>term2</t>
+          <t>term3</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -17607,42 +17925,42 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>100214</v>
+        <v>100213</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Daisey</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Flower</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D9" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>term3</t>
+          <t>term4</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>100214</v>
+        <v>100213</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Daisey</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Flower</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D10" s="38" t="n">
@@ -17650,25 +17968,25 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>term4</t>
+          <t>term1</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>100215</v>
+        <v>100213</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>XXX</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D11" s="38" t="n">
@@ -17676,25 +17994,25 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>term1</t>
+          <t>term2</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>100215</v>
+        <v>100213</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>XXX</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D12" s="38" t="n">
@@ -17702,25 +18020,25 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>term2</t>
+          <t>term3</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>100215</v>
+        <v>100213</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>XXX</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D13" s="38" t="n">
@@ -17728,111 +18046,111 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>term3</t>
+          <t>term4</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>100215</v>
+        <v>100214</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>XXX</t>
+          <t>Daisey</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Flower</t>
         </is>
       </c>
       <c r="D14" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>term4</t>
+          <t>term1</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>100216</v>
+        <v>100214</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>sadfasdf</t>
+          <t>Daisey</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Flower</t>
         </is>
       </c>
       <c r="D15" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>term1</t>
+          <t>term2</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>100216</v>
+        <v>100214</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>sadfasdf</t>
+          <t>Daisey</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Flower</t>
         </is>
       </c>
       <c r="D16" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>term2</t>
+          <t>term3</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>100216</v>
+        <v>100214</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>sadfasdf</t>
+          <t>Daisey</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Flower</t>
         </is>
       </c>
       <c r="D17" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>term3</t>
+          <t>term4</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -17841,16 +18159,16 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>100216</v>
+        <v>100214</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>sadfasdf</t>
+          <t>Daisey</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Flower</t>
         </is>
       </c>
       <c r="D18" s="38" t="n">
@@ -17858,20 +18176,20 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>term4</t>
+          <t>term1</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>100217</v>
+        <v>100214</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>asdfasdf</t>
+          <t>Daisey</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -17884,20 +18202,20 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>term1</t>
+          <t>term2</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>100217</v>
+        <v>100214</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>asdfasdf</t>
+          <t>Daisey</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -17910,20 +18228,20 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>term2</t>
+          <t>term3</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>100217</v>
+        <v>100214</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>asdfasdf</t>
+          <t>Daisey</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -17936,129 +18254,129 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>term3</t>
+          <t>term4</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>100217</v>
+        <v>100215</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>asdfasdf</t>
+          <t>XXX</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Flower</t>
+          <t>pppppppppppppppp</t>
         </is>
       </c>
       <c r="D22" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>term4</t>
+          <t>term1</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>100218</v>
+        <v>100215</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>XXX</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>pppppppppppppppp</t>
         </is>
       </c>
       <c r="D23" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>term1</t>
+          <t>term2</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>100218</v>
+        <v>100215</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>XXX</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>pppppppppppppppp</t>
         </is>
       </c>
       <c r="D24" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>term2</t>
+          <t>term3</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>100218</v>
+        <v>100215</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>XXX</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>pppppppppppppppp</t>
         </is>
       </c>
       <c r="D25" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>term3</t>
+          <t>term4</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>100218</v>
+        <v>100215</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>XXX</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>pppppppppppppppp</t>
         </is>
       </c>
       <c r="D26" s="38" t="n">
@@ -18066,25 +18384,25 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>term4</t>
+          <t>term1</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>100219</v>
+        <v>100215</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Daisey</t>
+          <t>XXX</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Flower</t>
+          <t>pppppppppppppppp</t>
         </is>
       </c>
       <c r="D27" s="38" t="n">
@@ -18092,25 +18410,25 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>term1</t>
+          <t>term2</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>100219</v>
+        <v>100215</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Daisey</t>
+          <t>XXX</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Flower</t>
+          <t>pppppppppppppppp</t>
         </is>
       </c>
       <c r="D28" s="38" t="n">
@@ -18118,25 +18436,25 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>term2</t>
+          <t>term3</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>100219</v>
+        <v>100215</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Daisey</t>
+          <t>XXX</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Flower</t>
+          <t>pppppppppppppppp</t>
         </is>
       </c>
       <c r="D29" s="38" t="n">
@@ -18144,46 +18462,46 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>term3</t>
+          <t>term4</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>100219</v>
+        <v>100216</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Daisey</t>
+          <t>sadfasdf</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Flower</t>
+          <t>pppppppppppppppp</t>
         </is>
       </c>
       <c r="D30" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>term4</t>
+          <t>term1</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>100220</v>
+        <v>100216</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>XXX</t>
+          <t>sadfasdf</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -18192,11 +18510,11 @@
         </is>
       </c>
       <c r="D31" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>term1</t>
+          <t>term2</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -18205,11 +18523,11 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>100220</v>
+        <v>100216</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>XXX</t>
+          <t>sadfasdf</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -18218,24 +18536,24 @@
         </is>
       </c>
       <c r="D32" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>term2</t>
+          <t>term3</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>100220</v>
+        <v>100216</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>XXX</t>
+          <t>sadfasdf</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -18244,24 +18562,24 @@
         </is>
       </c>
       <c r="D33" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>term3</t>
+          <t>term4</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>100220</v>
+        <v>100216</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>XXX</t>
+          <t>sadfasdf</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -18274,16 +18592,16 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>term4</t>
+          <t>term1</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>100221</v>
+        <v>100216</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -18300,16 +18618,16 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>term1</t>
+          <t>term2</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>100221</v>
+        <v>100216</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -18326,16 +18644,16 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>term2</t>
+          <t>term3</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>100221</v>
+        <v>100216</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -18352,42 +18670,42 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>term3</t>
+          <t>term4</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>100221</v>
+        <v>100217</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>sadfasdf</t>
+          <t>asdfasdf</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Flower</t>
         </is>
       </c>
       <c r="D38" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>term4</t>
+          <t>term1</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>100222</v>
+        <v>100217</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -18400,20 +18718,20 @@
         </is>
       </c>
       <c r="D39" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>term1</t>
+          <t>term2</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>100222</v>
+        <v>100217</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -18426,11 +18744,11 @@
         </is>
       </c>
       <c r="D40" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>term2</t>
+          <t>term3</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -18439,7 +18757,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>100222</v>
+        <v>100217</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -18452,20 +18770,20 @@
         </is>
       </c>
       <c r="D41" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>term3</t>
+          <t>term4</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>100222</v>
+        <v>100217</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -18482,25 +18800,25 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>term4</t>
+          <t>term1</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>100223</v>
+        <v>100217</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>asdfasdf</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Flower</t>
         </is>
       </c>
       <c r="D43" s="38" t="n">
@@ -18508,25 +18826,25 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>term1</t>
+          <t>term2</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>100223</v>
+        <v>100217</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>asdfasdf</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Flower</t>
         </is>
       </c>
       <c r="D44" s="38" t="n">
@@ -18534,25 +18852,25 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>term2</t>
+          <t>term3</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>100223</v>
+        <v>100217</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>asdfasdf</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Flower</t>
         </is>
       </c>
       <c r="D45" s="38" t="n">
@@ -18560,16 +18878,16 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>term3</t>
+          <t>term4</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>100223</v>
+        <v>100218</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -18582,89 +18900,89 @@
         </is>
       </c>
       <c r="D46" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>term4</t>
+          <t>term1</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>100224</v>
+        <v>100218</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Daisey</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Flower</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D47" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>term1</t>
+          <t>term2</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>100224</v>
+        <v>100218</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Daisey</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Flower</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D48" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>term2</t>
+          <t>term3</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>100224</v>
+        <v>100218</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Daisey</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Flower</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D49" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>term3</t>
+          <t>term4</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -18673,16 +18991,16 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>100224</v>
+        <v>100218</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Daisey</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Flower</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D50" s="38" t="n">
@@ -18690,25 +19008,25 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>term4</t>
+          <t>term1</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>100225</v>
+        <v>100218</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>XXX</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D51" s="38" t="n">
@@ -18716,25 +19034,25 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>term1</t>
+          <t>term2</t>
         </is>
       </c>
       <c r="F51" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>100225</v>
+        <v>100218</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>XXX</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D52" s="38" t="n">
@@ -18742,25 +19060,25 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>term2</t>
+          <t>term3</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>100225</v>
+        <v>100218</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>XXX</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D53" s="38" t="n">
@@ -18768,129 +19086,129 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>term3</t>
+          <t>term4</t>
         </is>
       </c>
       <c r="F53" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>100225</v>
+        <v>100219</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>XXX</t>
+          <t>Daisey</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Flower</t>
         </is>
       </c>
       <c r="D54" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>term4</t>
+          <t>term1</t>
         </is>
       </c>
       <c r="F54" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>100226</v>
+        <v>100219</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>sadfasdf</t>
+          <t>Daisey</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Flower</t>
         </is>
       </c>
       <c r="D55" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>term1</t>
+          <t>term2</t>
         </is>
       </c>
       <c r="F55" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>100226</v>
+        <v>100219</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>sadfasdf</t>
+          <t>Daisey</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Flower</t>
         </is>
       </c>
       <c r="D56" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>term2</t>
+          <t>term3</t>
         </is>
       </c>
       <c r="F56" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>100226</v>
+        <v>100219</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>sadfasdf</t>
+          <t>Daisey</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Flower</t>
         </is>
       </c>
       <c r="D57" s="38" t="n">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>term3</t>
+          <t>term4</t>
         </is>
       </c>
       <c r="F57" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>100226</v>
+        <v>100219</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>sadfasdf</t>
+          <t>Daisey</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>pppppppppppppppp</t>
+          <t>Flower</t>
         </is>
       </c>
       <c r="D58" s="38" t="n">
@@ -18898,20 +19216,20 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>term4</t>
+          <t>term1</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>100227</v>
+        <v>100219</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>asdfasdf</t>
+          <t>Daisey</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -18924,20 +19242,20 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>term1</t>
+          <t>term2</t>
         </is>
       </c>
       <c r="F59" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>100227</v>
+        <v>100219</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>asdfasdf</t>
+          <t>Daisey</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -18950,20 +19268,20 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>term2</t>
+          <t>term3</t>
         </is>
       </c>
       <c r="F60" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>100227</v>
+        <v>100219</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>asdfasdf</t>
+          <t>Daisey</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -18976,37 +19294,1779 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>term3</t>
+          <t>term4</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
+        <v>100220</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D62" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>100220</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D63" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>100220</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D64" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>100220</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D65" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>term4</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>100220</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D66" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>100220</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D67" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>100220</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D68" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>100220</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D69" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>term4</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>100221</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>sadfasdf</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D70" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>100221</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>sadfasdf</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D71" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>100221</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>sadfasdf</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D72" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>100221</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>sadfasdf</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D73" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>term4</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>100221</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>sadfasdf</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D74" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F74" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>100221</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>sadfasdf</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D75" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>100221</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>sadfasdf</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D76" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>100221</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>sadfasdf</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D77" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>term4</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>100222</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D78" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>100222</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D79" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>100222</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D80" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>100222</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D81" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>term4</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>100222</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D82" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>100222</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D83" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>100222</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D84" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>100222</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D85" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>term4</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>100223</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D86" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>100223</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D87" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>100223</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D88" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>100223</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D89" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>term4</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>100223</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D90" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>100223</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D91" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>100223</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D92" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>100223</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D93" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>term4</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>100224</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Daisey</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D94" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>100224</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Daisey</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D95" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>100224</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Daisey</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D96" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>100224</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Daisey</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D97" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>term4</t>
+        </is>
+      </c>
+      <c r="F97" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>100224</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Daisey</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D98" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F98" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>100224</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Daisey</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D99" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F99" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>100224</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Daisey</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D100" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F100" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100224</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Daisey</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D101" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>term4</t>
+        </is>
+      </c>
+      <c r="F101" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>100225</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D102" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F102" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>100225</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D103" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>100225</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D104" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F104" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>100225</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D105" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>term4</t>
+        </is>
+      </c>
+      <c r="F105" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>100225</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D106" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>100225</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D107" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>100225</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D108" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>100225</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D109" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>term4</t>
+        </is>
+      </c>
+      <c r="F109" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>100226</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>sadfasdf</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D110" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F110" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>100226</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>sadfasdf</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D111" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F111" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>100226</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>sadfasdf</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D112" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F112" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>100226</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>sadfasdf</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D113" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>term4</t>
+        </is>
+      </c>
+      <c r="F113" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>100226</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>sadfasdf</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D114" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>100226</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>sadfasdf</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D115" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F115" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>100226</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>sadfasdf</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D116" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>100226</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>sadfasdf</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>pppppppppppppppp</t>
+        </is>
+      </c>
+      <c r="D117" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>term4</t>
+        </is>
+      </c>
+      <c r="F117" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
         <v>100227</v>
       </c>
-      <c r="B62" t="inlineStr">
+      <c r="B118" t="inlineStr">
         <is>
           <t>asdfasdf</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="C118" t="inlineStr">
         <is>
           <t>Flower</t>
         </is>
       </c>
-      <c r="D62" s="38" t="n">
+      <c r="D118" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F118" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>100227</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D119" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F119" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>100227</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D120" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>100227</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D121" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>term4</t>
+        </is>
+      </c>
+      <c r="F121" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>100227</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D122" s="38" t="n">
         <v>44196</v>
       </c>
-      <c r="E62" t="inlineStr">
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>100227</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D123" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>100227</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D124" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>100227</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="D125" s="38" t="n">
+        <v>44196</v>
+      </c>
+      <c r="E125" t="inlineStr">
         <is>
           <t>term4</t>
         </is>
       </c>
-      <c r="F62" t="n">
+      <c r="F125" t="n">
         <v>20</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>100228</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>hhhhh</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>hhhhh</t>
+        </is>
+      </c>
+      <c r="D126" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>term1</t>
+        </is>
+      </c>
+      <c r="F126" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>100228</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>hhhhh</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>hhhhh</t>
+        </is>
+      </c>
+      <c r="D127" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>term2</t>
+        </is>
+      </c>
+      <c r="F127" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>100228</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>hhhhh</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>hhhhh</t>
+        </is>
+      </c>
+      <c r="D128" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>term3</t>
+        </is>
+      </c>
+      <c r="F128" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>100228</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>hhhhh</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>hhhhh</t>
+        </is>
+      </c>
+      <c r="D129" s="38" t="n">
+        <v>44561</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>term4</t>
+        </is>
+      </c>
+      <c r="F129" t="n">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>